<commit_message>
Variable Changed , Export updated and Results files updated
</commit_message>
<xml_diff>
--- a/Exports/CompleteResult.xlsx
+++ b/Exports/CompleteResult.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="26">
   <si>
     <t>Index</t>
   </si>
@@ -22,7 +22,16 @@
     <t>Time</t>
   </si>
   <si>
-    <t>Tavg [°C]</t>
+    <t>Tamb [°C]</t>
+  </si>
+  <si>
+    <t>Tmcooling [°C]</t>
+  </si>
+  <si>
+    <t>Tm [°C]</t>
+  </si>
+  <si>
+    <t>T heatflux [°C]</t>
   </si>
   <si>
     <t>Power [W]</t>
@@ -37,6 +46,9 @@
     <t>ideal elec. energy yield [Wh]</t>
   </si>
   <si>
+    <t>Performance Ratio [-]</t>
+  </si>
+  <si>
     <t>Performance Ratio STC[-]</t>
   </si>
   <si>
@@ -55,13 +67,7 @@
     <t>HP_Thermal[Wh]</t>
   </si>
   <si>
-    <t>Tamb</t>
-  </si>
-  <si>
     <t>E_sdp_eff</t>
-  </si>
-  <si>
-    <t>T_out</t>
   </si>
   <si>
     <t>P_fan</t>
@@ -447,13 +453,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:X19"/>
+  <dimension ref="A1:Z20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:26">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -523,1138 +529,1234 @@
       <c r="X1" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="Y1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:26">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>5548</v>
+        <v>8</v>
       </c>
       <c r="C2" s="2">
-        <v>41140.16597222222</v>
+        <v>40909.33333333334</v>
       </c>
       <c r="D2">
-        <v>20.64</v>
+        <v>11.35</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>11.57</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>11.67</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>11.61</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>33.2</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="J2">
-        <v>0</v>
+        <v>14.41</v>
       </c>
       <c r="K2">
-        <v>0</v>
+        <v>36.68</v>
       </c>
       <c r="L2">
         <v>0</v>
       </c>
       <c r="M2">
-        <v>9.15</v>
+        <v>0</v>
       </c>
       <c r="N2">
-        <v>622.2</v>
+        <v>0</v>
       </c>
       <c r="O2">
-        <v>20.64</v>
+        <v>0</v>
       </c>
       <c r="P2">
         <v>0</v>
       </c>
       <c r="Q2">
-        <v>20.64</v>
+        <v>10.27</v>
       </c>
       <c r="R2">
-        <v>0</v>
+        <v>698.36</v>
       </c>
       <c r="S2">
-        <v>0</v>
+        <v>12.57</v>
       </c>
       <c r="T2">
-        <v>0</v>
+        <v>29.71503191153772</v>
       </c>
       <c r="U2">
-        <v>0</v>
-      </c>
-      <c r="V2" t="s">
-        <v>23</v>
+        <v>0.3842016</v>
+      </c>
+      <c r="V2">
+        <v>0.007</v>
       </c>
       <c r="W2">
-        <v>0</v>
-      </c>
-      <c r="X2">
+        <v>43.75</v>
+      </c>
+      <c r="X2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:24">
+    <row r="3" spans="1:26">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>5549</v>
+        <v>9</v>
       </c>
       <c r="C3" s="2">
-        <v>41140.20763888889</v>
+        <v>40909.375</v>
       </c>
       <c r="D3">
-        <v>21.52927204673927</v>
+        <v>11.62</v>
       </c>
       <c r="E3">
-        <v>55.48</v>
+        <v>12.43</v>
       </c>
       <c r="F3">
-        <v>28</v>
+        <v>12.81</v>
       </c>
       <c r="G3">
-        <v>13.76</v>
+        <v>12.46</v>
       </c>
       <c r="H3">
-        <v>60.47</v>
+        <v>141.15</v>
       </c>
       <c r="I3">
-        <v>0.32</v>
+        <v>67</v>
       </c>
       <c r="J3">
-        <v>0.32</v>
+        <v>14.63</v>
       </c>
       <c r="K3">
-        <v>0.01</v>
+        <v>146.77</v>
       </c>
       <c r="L3">
-        <v>40.26</v>
+        <v>0.74</v>
       </c>
       <c r="M3">
-        <v>9.050000000000001</v>
+        <v>0.7</v>
       </c>
       <c r="N3">
-        <v>615.4</v>
+        <v>0.7</v>
       </c>
       <c r="O3">
-        <v>21.11</v>
+        <v>0.05</v>
       </c>
       <c r="P3">
-        <v>22.19</v>
+        <v>76.90000000000001</v>
       </c>
       <c r="Q3">
-        <v>21.51623696497774</v>
+        <v>10.16</v>
       </c>
       <c r="R3">
-        <v>31.91796050961846</v>
+        <v>690.88</v>
       </c>
       <c r="S3">
+        <v>52.51</v>
+      </c>
+      <c r="T3">
+        <v>29.90901708002477</v>
+      </c>
+      <c r="U3">
         <v>0.3842016</v>
       </c>
-      <c r="T3">
-        <v>0.011</v>
-      </c>
-      <c r="U3">
-        <v>39.29</v>
-      </c>
-      <c r="V3" t="s">
-        <v>23</v>
+      <c r="V3">
+        <v>0.023</v>
       </c>
       <c r="W3">
-        <v>0</v>
-      </c>
-      <c r="X3">
+        <v>34.33</v>
+      </c>
+      <c r="X3" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y3">
+        <v>0</v>
+      </c>
+      <c r="Z3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:24">
+    <row r="4" spans="1:26">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>5550</v>
+        <v>10</v>
       </c>
       <c r="C4" s="2">
-        <v>41140.24930555555</v>
+        <v>40909.41666666666</v>
       </c>
       <c r="D4">
-        <v>22.80880774224953</v>
+        <v>11.87</v>
       </c>
       <c r="E4">
-        <v>172.11</v>
+        <v>12.84</v>
       </c>
       <c r="F4">
-        <v>85</v>
+        <v>13.32</v>
       </c>
       <c r="G4">
-        <v>14.06</v>
+        <v>12.85</v>
       </c>
       <c r="H4">
-        <v>178.48</v>
+        <v>167.4</v>
       </c>
       <c r="I4">
+        <v>79</v>
+      </c>
+      <c r="J4">
+        <v>14.72</v>
+      </c>
+      <c r="K4">
+        <v>172.91</v>
+      </c>
+      <c r="L4">
         <v>0.75</v>
       </c>
-      <c r="J4">
-        <v>0.76</v>
-      </c>
-      <c r="K4">
+      <c r="M4">
+        <v>0.75</v>
+      </c>
+      <c r="N4">
+        <v>0.75</v>
+      </c>
+      <c r="O4">
         <v>0.06</v>
       </c>
-      <c r="L4">
-        <v>186.24</v>
-      </c>
-      <c r="M4">
-        <v>8.92</v>
-      </c>
-      <c r="N4">
-        <v>606.5599999999999</v>
-      </c>
-      <c r="O4">
-        <v>21.59</v>
-      </c>
       <c r="P4">
-        <v>67.09999999999999</v>
+        <v>88.43000000000001</v>
       </c>
       <c r="Q4">
-        <v>22.65200387654789</v>
+        <v>10.11</v>
       </c>
       <c r="R4">
-        <v>32.18450290506866</v>
+        <v>687.48</v>
       </c>
       <c r="S4">
+        <v>61.84</v>
+      </c>
+      <c r="T4">
+        <v>29.99541175831767</v>
+      </c>
+      <c r="U4">
         <v>0.3842016</v>
       </c>
-      <c r="T4">
-        <v>0.028</v>
-      </c>
-      <c r="U4">
-        <v>32.94</v>
-      </c>
-      <c r="V4" t="s">
-        <v>23</v>
+      <c r="V4">
+        <v>0.026</v>
       </c>
       <c r="W4">
-        <v>1</v>
-      </c>
-      <c r="X4">
+        <v>32.91</v>
+      </c>
+      <c r="X4" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y4">
+        <v>0</v>
+      </c>
+      <c r="Z4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:26">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>5551</v>
+        <v>11</v>
       </c>
       <c r="C5" s="2">
-        <v>41140.29097222222</v>
+        <v>40909.45833333334</v>
       </c>
       <c r="D5">
-        <v>27.02946972159518</v>
+        <v>12.12</v>
       </c>
       <c r="E5">
-        <v>395.56</v>
+        <v>13.26</v>
       </c>
       <c r="F5">
-        <v>192</v>
+        <v>13.84</v>
       </c>
       <c r="G5">
-        <v>14.31</v>
+        <v>13.25</v>
       </c>
       <c r="H5">
-        <v>397.02</v>
+        <v>195.52</v>
       </c>
       <c r="I5">
-        <v>0.89</v>
+        <v>92</v>
       </c>
       <c r="J5">
-        <v>0.9</v>
+        <v>14.76</v>
       </c>
       <c r="K5">
-        <v>0.17</v>
+        <v>200.76</v>
       </c>
       <c r="L5">
-        <v>321.48</v>
+        <v>0.86</v>
       </c>
       <c r="M5">
-        <v>8.44</v>
+        <v>0.78</v>
       </c>
       <c r="N5">
-        <v>573.92</v>
+        <v>0.78</v>
       </c>
       <c r="O5">
-        <v>24.48</v>
+        <v>0.08</v>
       </c>
       <c r="P5">
-        <v>151.09</v>
+        <v>98.8</v>
       </c>
       <c r="Q5">
-        <v>26.76852626229243</v>
+        <v>10.06</v>
       </c>
       <c r="R5">
-        <v>32.90116568827695</v>
+        <v>684.08</v>
       </c>
       <c r="S5">
+        <v>71.98</v>
+      </c>
+      <c r="T5">
+        <v>30.08464724337378</v>
+      </c>
+      <c r="U5">
         <v>0.3842016</v>
       </c>
-      <c r="T5">
-        <v>0.061</v>
-      </c>
-      <c r="U5">
-        <v>31.77</v>
-      </c>
-      <c r="V5" t="s">
-        <v>23</v>
+      <c r="V5">
+        <v>0.03</v>
       </c>
       <c r="W5">
+        <v>32.61</v>
+      </c>
+      <c r="X5" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y5">
         <v>1</v>
       </c>
-      <c r="X5">
+      <c r="Z5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:24">
+    <row r="6" spans="1:26">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>5552</v>
+        <v>12</v>
       </c>
       <c r="C6" s="2">
-        <v>41140.33263888889</v>
+        <v>40909.5</v>
       </c>
       <c r="D6">
-        <v>31.78008380974699</v>
+        <v>12.38</v>
       </c>
       <c r="E6">
-        <v>724.72</v>
+        <v>13.73</v>
       </c>
       <c r="F6">
-        <v>352</v>
+        <v>14.42</v>
       </c>
       <c r="G6">
-        <v>14.3</v>
+        <v>13.68</v>
       </c>
       <c r="H6">
-        <v>711.89</v>
+        <v>226.8</v>
       </c>
       <c r="I6">
-        <v>0.95</v>
+        <v>107</v>
       </c>
       <c r="J6">
-        <v>0.96</v>
+        <v>14.72</v>
       </c>
       <c r="K6">
-        <v>0.33</v>
+        <v>231.58</v>
       </c>
       <c r="L6">
-        <v>483.7</v>
+        <v>0.84</v>
       </c>
       <c r="M6">
-        <v>7.92</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="N6">
-        <v>538.5599999999999</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="O6">
-        <v>27.38</v>
+        <v>0.09</v>
       </c>
       <c r="P6">
-        <v>277.03</v>
+        <v>111.62</v>
       </c>
       <c r="Q6">
-        <v>31.50621552136363</v>
+        <v>10.01</v>
       </c>
       <c r="R6">
-        <v>34.02303348176625</v>
+        <v>680.6799999999999</v>
       </c>
       <c r="S6">
+        <v>83.76000000000001</v>
+      </c>
+      <c r="T6">
+        <v>30.18179078262646</v>
+      </c>
+      <c r="U6">
         <v>0.3842016</v>
       </c>
-      <c r="T6">
-        <v>0.111</v>
-      </c>
-      <c r="U6">
-        <v>31.53</v>
-      </c>
-      <c r="V6" t="s">
-        <v>23</v>
+      <c r="V6">
+        <v>0.035</v>
       </c>
       <c r="W6">
+        <v>32.71</v>
+      </c>
+      <c r="X6" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y6">
         <v>1</v>
       </c>
-      <c r="X6">
+      <c r="Z6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:24">
+    <row r="7" spans="1:26">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>5553</v>
+        <v>13</v>
       </c>
       <c r="C7" s="2">
-        <v>41140.37430555555</v>
+        <v>40909.54166666666</v>
       </c>
       <c r="D7">
-        <v>36.59493695867236</v>
+        <v>12.38</v>
       </c>
       <c r="E7">
-        <v>1073.8</v>
+        <v>12.62</v>
       </c>
       <c r="F7">
-        <v>525</v>
+        <v>12.72</v>
       </c>
       <c r="G7">
-        <v>14.2</v>
+        <v>12.65</v>
       </c>
       <c r="H7">
-        <v>1041.71</v>
+        <v>34.99</v>
       </c>
       <c r="I7">
-        <v>0.98</v>
+        <v>17</v>
       </c>
       <c r="J7">
-        <v>0.99</v>
+        <v>14.29</v>
       </c>
       <c r="K7">
-        <v>0.49</v>
+        <v>38.61</v>
       </c>
       <c r="L7">
-        <v>646.63</v>
+        <v>0</v>
       </c>
       <c r="M7">
-        <v>7.4</v>
+        <v>0</v>
       </c>
       <c r="N7">
-        <v>503.2</v>
+        <v>0</v>
       </c>
       <c r="O7">
-        <v>30.28</v>
+        <v>0</v>
       </c>
       <c r="P7">
-        <v>413.68</v>
+        <v>0</v>
       </c>
       <c r="Q7">
-        <v>36.39784012268746</v>
+        <v>10.14</v>
       </c>
       <c r="R7">
-        <v>35.20275813843804</v>
+        <v>689.52</v>
       </c>
       <c r="S7">
+        <v>13.38</v>
+      </c>
+      <c r="T7">
+        <v>29.94292480675038</v>
+      </c>
+      <c r="U7">
         <v>0.3842016</v>
       </c>
-      <c r="T7">
-        <v>0.164</v>
-      </c>
-      <c r="U7">
-        <v>31.24</v>
-      </c>
-      <c r="V7" t="s">
-        <v>23</v>
+      <c r="V7">
+        <v>0.007</v>
       </c>
       <c r="W7">
-        <v>1</v>
-      </c>
-      <c r="X7">
+        <v>41.18</v>
+      </c>
+      <c r="X7" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y7">
+        <v>0</v>
+      </c>
+      <c r="Z7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:24">
+    <row r="8" spans="1:26">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>5554</v>
+        <v>14</v>
       </c>
       <c r="C8" s="2">
-        <v>41140.41597222222</v>
+        <v>40909.58333333334</v>
       </c>
       <c r="D8">
-        <v>39.55622569701902</v>
+        <v>12.39</v>
       </c>
       <c r="E8">
-        <v>1377.99</v>
+        <v>12.94</v>
       </c>
       <c r="F8">
-        <v>677</v>
+        <v>13.2</v>
       </c>
       <c r="G8">
-        <v>14.13</v>
+        <v>12.95</v>
       </c>
       <c r="H8">
-        <v>1327.55</v>
+        <v>86.02</v>
       </c>
       <c r="I8">
-        <v>0.99</v>
+        <v>42</v>
       </c>
       <c r="J8">
-        <v>1</v>
+        <v>14.22</v>
       </c>
       <c r="K8">
-        <v>0.63</v>
+        <v>91.31999999999999</v>
       </c>
       <c r="L8">
-        <v>801.23</v>
+        <v>0.47</v>
       </c>
       <c r="M8">
-        <v>7.1</v>
+        <v>0.54</v>
       </c>
       <c r="N8">
-        <v>482.8</v>
+        <v>0.54</v>
       </c>
       <c r="O8">
-        <v>31.44</v>
+        <v>0.02</v>
       </c>
       <c r="P8">
-        <v>533.92</v>
+        <v>36.48</v>
       </c>
       <c r="Q8">
-        <v>39.30836390911162</v>
+        <v>10.1</v>
       </c>
       <c r="R8">
-        <v>35.92187916037615</v>
+        <v>686.8</v>
       </c>
       <c r="S8">
+        <v>33.09</v>
+      </c>
+      <c r="T8">
+        <v>30.0119270869451</v>
+      </c>
+      <c r="U8">
         <v>0.3842016</v>
       </c>
-      <c r="T8">
-        <v>0.211</v>
-      </c>
-      <c r="U8">
-        <v>31.17</v>
-      </c>
-      <c r="V8" t="s">
-        <v>23</v>
+      <c r="V8">
+        <v>0.015</v>
       </c>
       <c r="W8">
-        <v>1</v>
-      </c>
-      <c r="X8">
+        <v>35.71</v>
+      </c>
+      <c r="X8" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y8">
+        <v>0</v>
+      </c>
+      <c r="Z8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:24">
+    <row r="9" spans="1:26">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>5555</v>
+        <v>15</v>
       </c>
       <c r="C9" s="2">
-        <v>41140.45763888889</v>
+        <v>40909.625</v>
       </c>
       <c r="D9">
-        <v>41.79465802910201</v>
+        <v>12.39</v>
       </c>
       <c r="E9">
-        <v>1553.47</v>
+        <v>12.39</v>
       </c>
       <c r="F9">
-        <v>768</v>
+        <v>12.39</v>
       </c>
       <c r="G9">
-        <v>14.05</v>
+        <v>12.39</v>
       </c>
       <c r="H9">
-        <v>1492.22</v>
+        <v>0</v>
       </c>
       <c r="I9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J9">
-        <v>1.01</v>
+        <v>0</v>
       </c>
       <c r="K9">
-        <v>0.72</v>
+        <v>0</v>
       </c>
       <c r="L9">
-        <v>913.5</v>
+        <v>0</v>
       </c>
       <c r="M9">
-        <v>6.88</v>
+        <v>0</v>
       </c>
       <c r="N9">
-        <v>467.84</v>
+        <v>0</v>
       </c>
       <c r="O9">
-        <v>32.6</v>
+        <v>0</v>
       </c>
       <c r="P9">
-        <v>606.36</v>
+        <v>0</v>
       </c>
       <c r="Q9">
-        <v>41.52254428354365</v>
+        <v>10.17</v>
       </c>
       <c r="R9">
-        <v>36.47003319711263</v>
+        <v>691.5599999999999</v>
       </c>
       <c r="S9">
-        <v>0.3842016</v>
+        <v>0</v>
       </c>
       <c r="T9">
-        <v>0.239</v>
+        <v>0</v>
       </c>
       <c r="U9">
-        <v>31.12</v>
-      </c>
-      <c r="V9" t="s">
-        <v>23</v>
+        <v>0</v>
+      </c>
+      <c r="V9">
+        <v>0</v>
       </c>
       <c r="W9">
-        <v>1</v>
-      </c>
-      <c r="X9">
+        <v>0</v>
+      </c>
+      <c r="X9" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y9">
+        <v>0</v>
+      </c>
+      <c r="Z9">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:24">
+    <row r="10" spans="1:26">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>5556</v>
+        <v>16</v>
       </c>
       <c r="C10" s="2">
-        <v>41140.49930555555</v>
+        <v>40909.66666666666</v>
       </c>
       <c r="D10">
-        <v>42.91391917402582</v>
+        <v>12.31</v>
       </c>
       <c r="E10">
-        <v>1538.72</v>
+        <v>12.31</v>
       </c>
       <c r="F10">
-        <v>764</v>
+        <v>12.31</v>
       </c>
       <c r="G10">
-        <v>13.99</v>
+        <v>12.31</v>
       </c>
       <c r="H10">
-        <v>1478.41</v>
+        <v>0</v>
       </c>
       <c r="I10">
-        <v>0.99</v>
+        <v>0</v>
       </c>
       <c r="J10">
-        <v>1.01</v>
+        <v>0</v>
       </c>
       <c r="K10">
-        <v>0.71</v>
+        <v>0</v>
       </c>
       <c r="L10">
-        <v>901.6799999999999</v>
+        <v>0</v>
       </c>
       <c r="M10">
-        <v>6.77</v>
+        <v>0</v>
       </c>
       <c r="N10">
-        <v>460.36</v>
+        <v>0</v>
       </c>
       <c r="O10">
-        <v>33.76</v>
+        <v>0</v>
       </c>
       <c r="P10">
-        <v>603.66</v>
+        <v>0</v>
       </c>
       <c r="Q10">
-        <v>42.64386786003314</v>
+        <v>10.18</v>
       </c>
       <c r="R10">
-        <v>36.74159439858167</v>
+        <v>692.24</v>
       </c>
       <c r="S10">
-        <v>0.3842016</v>
+        <v>0</v>
       </c>
       <c r="T10">
-        <v>0.238</v>
+        <v>0</v>
       </c>
       <c r="U10">
-        <v>31.15</v>
-      </c>
-      <c r="V10" t="s">
-        <v>23</v>
+        <v>0</v>
+      </c>
+      <c r="V10">
+        <v>0</v>
       </c>
       <c r="W10">
-        <v>1</v>
-      </c>
-      <c r="X10">
+        <v>0</v>
+      </c>
+      <c r="X10" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y10">
+        <v>0</v>
+      </c>
+      <c r="Z10">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:24">
+    <row r="11" spans="1:26">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11">
-        <v>5557</v>
+        <v>17</v>
       </c>
       <c r="C11" s="2">
-        <v>41140.54097222222</v>
+        <v>40909.70833333334</v>
       </c>
       <c r="D11">
-        <v>42.47030915801759</v>
+        <v>12.23</v>
       </c>
       <c r="E11">
-        <v>1349.72</v>
+        <v>12.23</v>
       </c>
       <c r="F11">
-        <v>671</v>
+        <v>12.23</v>
       </c>
       <c r="G11">
-        <v>13.97</v>
+        <v>12.23</v>
       </c>
       <c r="H11">
-        <v>1301.1</v>
+        <v>0</v>
       </c>
       <c r="I11">
-        <v>0.99</v>
+        <v>0</v>
       </c>
       <c r="J11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K11">
-        <v>0.62</v>
+        <v>0</v>
       </c>
       <c r="L11">
-        <v>848.71</v>
+        <v>0</v>
       </c>
       <c r="M11">
-        <v>6.85</v>
+        <v>0</v>
       </c>
       <c r="N11">
-        <v>465.8</v>
+        <v>0</v>
       </c>
       <c r="O11">
-        <v>33.99</v>
+        <v>0</v>
       </c>
       <c r="P11">
-        <v>530.3</v>
+        <v>0</v>
       </c>
       <c r="Q11">
-        <v>41.80934062905709</v>
+        <v>10.19</v>
       </c>
       <c r="R11">
-        <v>36.52411564382545</v>
+        <v>692.92</v>
       </c>
       <c r="S11">
-        <v>0.3842016</v>
+        <v>0</v>
       </c>
       <c r="T11">
-        <v>0.21</v>
+        <v>0</v>
       </c>
       <c r="U11">
-        <v>31.3</v>
-      </c>
-      <c r="V11" t="s">
-        <v>23</v>
+        <v>0</v>
+      </c>
+      <c r="V11">
+        <v>0</v>
       </c>
       <c r="W11">
-        <v>1</v>
-      </c>
-      <c r="X11">
+        <v>0</v>
+      </c>
+      <c r="X11" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y11">
+        <v>0</v>
+      </c>
+      <c r="Z11">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:24">
+    <row r="12" spans="1:26">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12">
-        <v>5558</v>
+        <v>18</v>
       </c>
       <c r="C12" s="2">
-        <v>41140.58263888889</v>
+        <v>40909.75</v>
       </c>
       <c r="D12">
-        <v>41.16313742222992</v>
+        <v>12.15</v>
       </c>
       <c r="E12">
-        <v>1038.05</v>
+        <v>12.15</v>
       </c>
       <c r="F12">
-        <v>518</v>
+        <v>12.15</v>
       </c>
       <c r="G12">
-        <v>13.92</v>
+        <v>12.15</v>
       </c>
       <c r="H12">
-        <v>1008.41</v>
+        <v>0</v>
       </c>
       <c r="I12">
-        <v>0.97</v>
+        <v>0</v>
       </c>
       <c r="J12">
-        <v>0.99</v>
+        <v>0</v>
       </c>
       <c r="K12">
-        <v>0.47</v>
+        <v>0</v>
       </c>
       <c r="L12">
-        <v>721.66</v>
+        <v>0</v>
       </c>
       <c r="M12">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="N12">
-        <v>476</v>
+        <v>0</v>
       </c>
       <c r="O12">
-        <v>34.22</v>
+        <v>0</v>
       </c>
       <c r="P12">
-        <v>409.65</v>
+        <v>0</v>
       </c>
       <c r="Q12">
-        <v>40.28417660104788</v>
+        <v>10.2</v>
       </c>
       <c r="R12">
-        <v>36.13151436590128</v>
+        <v>693.6</v>
       </c>
       <c r="S12">
-        <v>0.3842016</v>
+        <v>0</v>
       </c>
       <c r="T12">
-        <v>0.163</v>
+        <v>0</v>
       </c>
       <c r="U12">
-        <v>31.47</v>
-      </c>
-      <c r="V12" t="s">
-        <v>23</v>
+        <v>0</v>
+      </c>
+      <c r="V12">
+        <v>0</v>
       </c>
       <c r="W12">
-        <v>1</v>
-      </c>
-      <c r="X12">
+        <v>0</v>
+      </c>
+      <c r="X12" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y12">
+        <v>0</v>
+      </c>
+      <c r="Z12">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:24">
+    <row r="13" spans="1:26">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13">
-        <v>5559</v>
+        <v>19</v>
       </c>
       <c r="C13" s="2">
-        <v>41140.62430555555</v>
+        <v>40909.79166666666</v>
       </c>
       <c r="D13">
-        <v>39.44001411660747</v>
+        <v>12.19</v>
       </c>
       <c r="E13">
-        <v>691.72</v>
+        <v>12.19</v>
       </c>
       <c r="F13">
-        <v>347</v>
+        <v>12.19</v>
       </c>
       <c r="G13">
-        <v>13.84</v>
+        <v>12.19</v>
       </c>
       <c r="H13">
-        <v>681.37</v>
+        <v>0</v>
       </c>
       <c r="I13">
-        <v>0.9399999999999999</v>
+        <v>0</v>
       </c>
       <c r="J13">
-        <v>0.96</v>
+        <v>0</v>
       </c>
       <c r="K13">
-        <v>0.31</v>
+        <v>0</v>
       </c>
       <c r="L13">
-        <v>497.63</v>
+        <v>0</v>
       </c>
       <c r="M13">
-        <v>7.18</v>
+        <v>0</v>
       </c>
       <c r="N13">
-        <v>488.24</v>
+        <v>0</v>
       </c>
       <c r="O13">
-        <v>34.45</v>
+        <v>0</v>
       </c>
       <c r="P13">
-        <v>274.67</v>
+        <v>0</v>
       </c>
       <c r="Q13">
-        <v>38.54759380987457</v>
+        <v>10.2</v>
       </c>
       <c r="R13">
-        <v>35.68734588438377</v>
+        <v>693.6</v>
       </c>
       <c r="S13">
-        <v>0.3842016</v>
+        <v>0</v>
       </c>
       <c r="T13">
-        <v>0.11</v>
+        <v>0</v>
       </c>
       <c r="U13">
-        <v>31.7</v>
-      </c>
-      <c r="V13" t="s">
-        <v>23</v>
+        <v>0</v>
+      </c>
+      <c r="V13">
+        <v>0</v>
       </c>
       <c r="W13">
-        <v>1</v>
-      </c>
-      <c r="X13">
+        <v>0</v>
+      </c>
+      <c r="X13" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y13">
+        <v>0</v>
+      </c>
+      <c r="Z13">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:24">
+    <row r="14" spans="1:26">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14">
-        <v>5560</v>
+        <v>20</v>
       </c>
       <c r="C14" s="2">
-        <v>41140.66597222222</v>
+        <v>40909.83333333334</v>
       </c>
       <c r="D14">
-        <v>35.75584529946498</v>
+        <v>12.23</v>
       </c>
       <c r="E14">
-        <v>380.74</v>
+        <v>12.23</v>
       </c>
       <c r="F14">
-        <v>192</v>
+        <v>12.23</v>
       </c>
       <c r="G14">
-        <v>13.77</v>
+        <v>12.23</v>
       </c>
       <c r="H14">
-        <v>383.77</v>
+        <v>0</v>
       </c>
       <c r="I14">
-        <v>0.88</v>
+        <v>0</v>
       </c>
       <c r="J14">
-        <v>0.89</v>
+        <v>0</v>
       </c>
       <c r="K14">
-        <v>0.16</v>
+        <v>0</v>
       </c>
       <c r="L14">
-        <v>262.38</v>
+        <v>0</v>
       </c>
       <c r="M14">
-        <v>7.53</v>
+        <v>0</v>
       </c>
       <c r="N14">
-        <v>512.04</v>
+        <v>0</v>
       </c>
       <c r="O14">
-        <v>32.82</v>
+        <v>0</v>
       </c>
       <c r="P14">
-        <v>152.12</v>
+        <v>0</v>
       </c>
       <c r="Q14">
-        <v>35.12885669595232</v>
+        <v>10.19</v>
       </c>
       <c r="R14">
-        <v>34.84909185877343</v>
+        <v>692.92</v>
       </c>
       <c r="S14">
-        <v>0.3842016</v>
+        <v>0</v>
       </c>
       <c r="T14">
-        <v>0.062</v>
+        <v>0</v>
       </c>
       <c r="U14">
-        <v>32.29</v>
-      </c>
-      <c r="V14" t="s">
-        <v>23</v>
+        <v>0</v>
+      </c>
+      <c r="V14">
+        <v>0</v>
       </c>
       <c r="W14">
-        <v>1</v>
-      </c>
-      <c r="X14">
+        <v>0</v>
+      </c>
+      <c r="X14" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y14">
+        <v>0</v>
+      </c>
+      <c r="Z14">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:24">
+    <row r="15" spans="1:26">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15">
-        <v>5561</v>
+        <v>21</v>
       </c>
       <c r="C15" s="2">
-        <v>41140.70763888889</v>
+        <v>40909.875</v>
       </c>
       <c r="D15">
-        <v>32.6141341456872</v>
+        <v>12.27</v>
       </c>
       <c r="E15">
-        <v>165.52</v>
+        <v>12.27</v>
       </c>
       <c r="F15">
-        <v>85</v>
+        <v>12.27</v>
       </c>
       <c r="G15">
-        <v>13.52</v>
+        <v>12.27</v>
       </c>
       <c r="H15">
-        <v>172.88</v>
+        <v>0</v>
       </c>
       <c r="I15">
-        <v>0.74</v>
+        <v>0</v>
       </c>
       <c r="J15">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="K15">
-        <v>0.06</v>
+        <v>0</v>
       </c>
       <c r="L15">
-        <v>91.55</v>
+        <v>0</v>
       </c>
       <c r="M15">
-        <v>7.83</v>
+        <v>0</v>
       </c>
       <c r="N15">
-        <v>532.4400000000001</v>
+        <v>0</v>
       </c>
       <c r="O15">
-        <v>31.2</v>
+        <v>0</v>
       </c>
       <c r="P15">
-        <v>67.56</v>
+        <v>0</v>
       </c>
       <c r="Q15">
-        <v>32.27376331303623</v>
+        <v>10.19</v>
       </c>
       <c r="R15">
-        <v>34.16014518196838</v>
+        <v>692.92</v>
       </c>
       <c r="S15">
-        <v>0.3842016</v>
+        <v>0</v>
       </c>
       <c r="T15">
-        <v>0.029</v>
+        <v>0</v>
       </c>
       <c r="U15">
-        <v>34.12</v>
-      </c>
-      <c r="V15" t="s">
-        <v>23</v>
+        <v>0</v>
+      </c>
+      <c r="V15">
+        <v>0</v>
       </c>
       <c r="W15">
         <v>0</v>
       </c>
-      <c r="X15">
+      <c r="X15" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y15">
+        <v>0</v>
+      </c>
+      <c r="Z15">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:24">
+    <row r="16" spans="1:26">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16">
-        <v>5562</v>
+        <v>22</v>
       </c>
       <c r="C16" s="2">
-        <v>41140.74930555555</v>
+        <v>40909.91666666666</v>
       </c>
       <c r="D16">
-        <v>29.91912043403099</v>
+        <v>12.18</v>
       </c>
       <c r="E16">
-        <v>36.23</v>
+        <v>12.18</v>
       </c>
       <c r="F16">
-        <v>19</v>
+        <v>12.18</v>
       </c>
       <c r="G16">
-        <v>13.24</v>
+        <v>12.18</v>
       </c>
       <c r="H16">
-        <v>40.65</v>
+        <v>0</v>
       </c>
       <c r="I16">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="J16">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="K16">
         <v>0</v>
       </c>
       <c r="L16">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="M16">
-        <v>8.09</v>
+        <v>0</v>
       </c>
       <c r="N16">
-        <v>550.12</v>
+        <v>0</v>
       </c>
       <c r="O16">
-        <v>29.57</v>
+        <v>0</v>
       </c>
       <c r="P16">
-        <v>15.15</v>
+        <v>0</v>
       </c>
       <c r="Q16">
-        <v>29.87792925412037</v>
+        <v>10.2</v>
       </c>
       <c r="R16">
-        <v>33.59110758542812</v>
+        <v>693.6</v>
       </c>
       <c r="S16">
-        <v>0.3842016</v>
+        <v>0</v>
       </c>
       <c r="T16">
-        <v>0.008</v>
+        <v>0</v>
       </c>
       <c r="U16">
-        <v>42.11</v>
-      </c>
-      <c r="V16" t="s">
-        <v>23</v>
+        <v>0</v>
+      </c>
+      <c r="V16">
+        <v>0</v>
       </c>
       <c r="W16">
         <v>0</v>
       </c>
-      <c r="X16">
+      <c r="X16" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y16">
+        <v>0</v>
+      </c>
+      <c r="Z16">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:24">
+    <row r="17" spans="1:26">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17">
-        <v>5563</v>
+        <v>23</v>
       </c>
       <c r="C17" s="2">
-        <v>41140.79097222222</v>
+        <v>40909.95833333334</v>
       </c>
       <c r="D17">
-        <v>27.97</v>
+        <v>12.1</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>12.1</v>
       </c>
       <c r="F17">
-        <v>0</v>
+        <v>12.1</v>
       </c>
       <c r="G17">
-        <v>0</v>
+        <v>12.1</v>
       </c>
       <c r="H17">
         <v>0</v>
@@ -1672,22 +1774,22 @@
         <v>0</v>
       </c>
       <c r="M17">
-        <v>8.31</v>
+        <v>0</v>
       </c>
       <c r="N17">
-        <v>565.08</v>
+        <v>0</v>
       </c>
       <c r="O17">
-        <v>27.97</v>
+        <v>0</v>
       </c>
       <c r="P17">
         <v>0</v>
       </c>
       <c r="Q17">
-        <v>27.97</v>
+        <v>10.21</v>
       </c>
       <c r="R17">
-        <v>0</v>
+        <v>694.28</v>
       </c>
       <c r="S17">
         <v>0</v>
@@ -1698,138 +1800,236 @@
       <c r="U17">
         <v>0</v>
       </c>
-      <c r="V17" t="s">
-        <v>23</v>
+      <c r="V17">
+        <v>0</v>
       </c>
       <c r="W17">
         <v>0</v>
       </c>
-      <c r="X17">
+      <c r="X17" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y17">
+        <v>0</v>
+      </c>
+      <c r="Z17">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:24">
+    <row r="18" spans="1:26">
       <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="B18">
-        <v>88888</v>
+        <v>24</v>
+      </c>
+      <c r="C18" s="2">
+        <v>40910</v>
       </c>
       <c r="D18">
-        <v>533.9799337551883</v>
+        <v>12.02</v>
       </c>
       <c r="E18">
-        <v>10553.83</v>
+        <v>12.02</v>
       </c>
       <c r="F18">
-        <v>5223</v>
+        <v>12.02</v>
       </c>
       <c r="G18">
-        <v>195.06</v>
+        <v>12.02</v>
       </c>
       <c r="H18">
-        <v>10275.93</v>
+        <v>0</v>
       </c>
       <c r="I18">
-        <v>11.4</v>
+        <v>0</v>
       </c>
       <c r="J18">
-        <v>11.55</v>
+        <v>0</v>
       </c>
       <c r="K18">
-        <v>4.74</v>
+        <v>0</v>
       </c>
       <c r="L18">
-        <v>6716.849999999999</v>
+        <v>0</v>
       </c>
       <c r="M18">
-        <v>124.42</v>
+        <v>0</v>
       </c>
       <c r="N18">
-        <v>8460.559999999999</v>
+        <v>0</v>
       </c>
       <c r="O18">
-        <v>467.5</v>
+        <v>0</v>
       </c>
       <c r="P18">
-        <v>4124.48</v>
+        <v>0</v>
       </c>
       <c r="Q18">
-        <v>528.847259103646</v>
+        <v>10.22</v>
       </c>
       <c r="R18">
-        <v>486.3062479995193</v>
+        <v>694.96</v>
       </c>
       <c r="S18">
-        <v>5.3788224</v>
+        <v>0</v>
       </c>
       <c r="T18">
-        <v>1.645</v>
+        <v>0</v>
       </c>
       <c r="U18">
-        <v>463.2</v>
+        <v>0</v>
+      </c>
+      <c r="V18">
+        <v>0</v>
+      </c>
+      <c r="W18">
+        <v>0</v>
+      </c>
+      <c r="X18" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y18">
+        <v>0</v>
+      </c>
+      <c r="Z18">
+        <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:24">
+    <row r="19" spans="1:26">
       <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="B19">
-        <v>6349.142857142857</v>
+        <v>272</v>
       </c>
       <c r="D19">
-        <v>38.14142383965631</v>
+        <v>206.18</v>
       </c>
       <c r="E19">
-        <v>753.8449999999999</v>
+        <v>211.46</v>
       </c>
       <c r="F19">
-        <v>373.0714285714286</v>
+        <v>214.05</v>
       </c>
       <c r="G19">
-        <v>13.93285714285714</v>
+        <v>211.52</v>
       </c>
       <c r="H19">
-        <v>733.995</v>
+        <v>885.0799999999999</v>
       </c>
       <c r="I19">
-        <v>0.8142857142857142</v>
+        <v>420</v>
       </c>
       <c r="J19">
-        <v>0.825</v>
+        <v>101.75</v>
       </c>
       <c r="K19">
-        <v>0.3385714285714286</v>
+        <v>918.63</v>
       </c>
       <c r="L19">
-        <v>479.775</v>
+        <v>3.66</v>
       </c>
       <c r="M19">
-        <v>8.887142857142857</v>
+        <v>3.58</v>
       </c>
       <c r="N19">
-        <v>604.3257142857143</v>
+        <v>3.58</v>
       </c>
       <c r="O19">
-        <v>33.39285714285715</v>
+        <v>0.3</v>
       </c>
       <c r="P19">
-        <v>294.6057142857143</v>
+        <v>412.23</v>
       </c>
       <c r="Q19">
-        <v>37.774804221689</v>
+        <v>172.8</v>
       </c>
       <c r="R19">
-        <v>34.73616057139423</v>
+        <v>11750.4</v>
       </c>
       <c r="S19">
+        <v>329.13</v>
+      </c>
+      <c r="T19">
+        <v>209.8407506695759</v>
+      </c>
+      <c r="U19">
+        <v>2.6894112</v>
+      </c>
+      <c r="V19">
+        <v>0.143</v>
+      </c>
+      <c r="W19">
+        <v>253.2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>38.85714285714285</v>
+      </c>
+      <c r="D20">
+        <v>29.45428571428571</v>
+      </c>
+      <c r="E20">
+        <v>30.20857142857143</v>
+      </c>
+      <c r="F20">
+        <v>30.57857142857143</v>
+      </c>
+      <c r="G20">
+        <v>30.21714285714286</v>
+      </c>
+      <c r="H20">
+        <v>126.44</v>
+      </c>
+      <c r="I20">
+        <v>60</v>
+      </c>
+      <c r="J20">
+        <v>14.53571428571429</v>
+      </c>
+      <c r="K20">
+        <v>131.2328571428571</v>
+      </c>
+      <c r="L20">
+        <v>0.5228571428571428</v>
+      </c>
+      <c r="M20">
+        <v>0.5114285714285715</v>
+      </c>
+      <c r="N20">
+        <v>0.5114285714285715</v>
+      </c>
+      <c r="O20">
+        <v>0.04285714285714286</v>
+      </c>
+      <c r="P20">
+        <v>58.89</v>
+      </c>
+      <c r="Q20">
+        <v>24.68571428571428</v>
+      </c>
+      <c r="R20">
+        <v>1678.628571428571</v>
+      </c>
+      <c r="S20">
+        <v>47.01857142857143</v>
+      </c>
+      <c r="T20">
+        <v>29.97725009565369</v>
+      </c>
+      <c r="U20">
         <v>0.3842016</v>
       </c>
-      <c r="T19">
-        <v>0.1175</v>
-      </c>
-      <c r="U19">
-        <v>33.08571428571429</v>
+      <c r="V20">
+        <v>0.02042857142857143</v>
+      </c>
+      <c r="W20">
+        <v>36.17142857142857</v>
       </c>
     </row>
   </sheetData>

</xml_diff>